<commit_message>
Added Reference projects to README.md. Simplified EntityLicense and LicenseImporter class structure.
</commit_message>
<xml_diff>
--- a/Assets/Cucurbit/Easy License View/ExcelData/license.xlsx
+++ b/Assets/Cucurbit/Easy License View/ExcelData/license.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="licenses" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="license" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -33,6 +33,28 @@
   <si>
     <t xml:space="preserve">The MIT License (MIT)
 Copyright (c) 2018 xxxxxxxxxxxx
+Permission is hereby granted, free of charge, to any person obtaining a copy
+of this software and associated documentation files (the "Software"), to deal
+in the Software without restriction, including without limitation the rights
+to use, copy, modify, merge, publish, distribute, sublicense, and/or sell
+copies of the Software, and to permit persons to whom the Software is
+furnished to do so, subject to the following conditions:
+The above copyright notice and this permission notice shall be included in all
+copies or substantial portions of the Software.
+THE SOFTWARE IS PROVIDED "AS IS", WITHOUT WARRANTY OF ANY KIND, EXPRESS OR
+IMPLIED, INCLUDING BUT NOT LIMITED TO THE WARRANTIES OF MERCHANTABILITY,
+FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT. IN NO EVENT SHALL THE
+AUTHORS OR COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER
+LIABILITY, WHETHER IN AN ACTION OF CONTRACT, TORT OR OTHERWISE, ARISING FROM,
+OUT OF OR IN CONNECTION WITH THE SOFTWARE OR THE USE OR OTHER DEALINGS IN THE
+SOFTWARE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy License View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MIT License (MIT)
+Copyright (c) 2018 nakagawa akihiro
 Permission is hereby granted, free of charge, to any person obtaining a copy
 of this software and associated documentation files (the "Software"), to deal
 in the Software without restriction, including without limitation the rights
@@ -222,10 +244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -253,7 +275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -261,14 +283,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -290,6 +316,10 @@
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>